<commit_message>
Built libraries and BOM work
</commit_message>
<xml_diff>
--- a/boards/on-robot/control-v3.4/control-bom.xlsx
+++ b/boards/on-robot/control-v3.4/control-bom.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ber20\Documents\GitHub\robocup-pcb\boards\on-robot\control-v3.4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{83943F0A-BA20-4F14-9BB6-23DBF440E548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A05F1F-3440-4E0E-BC39-8C0D8617DA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="control-bom" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="161">
   <si>
     <t>Qty</t>
   </si>
@@ -40,12 +40,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Availability</t>
-  </si>
-  <si>
-    <t>Replacement/Action</t>
-  </si>
-  <si>
     <t>R-US_R0603</t>
   </si>
   <si>
@@ -58,9 +52,6 @@
     <t>RESISTOR, American symbol</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>0.022uF 50V</t>
   </si>
   <si>
@@ -154,9 +145,6 @@
     <t>Power Connector</t>
   </si>
   <si>
-    <t>Wires are directly soldered to control</t>
-  </si>
-  <si>
     <t>2.2uF 50V</t>
   </si>
   <si>
@@ -175,12 +163,6 @@
     <t>Surface Mount DIP Switch Series 219 SMT</t>
   </si>
   <si>
-    <t>Not needed, doesn't do anything</t>
-  </si>
-  <si>
-    <t>Remove</t>
-  </si>
-  <si>
     <t>22uF 16V</t>
   </si>
   <si>
@@ -253,9 +235,6 @@
     <t>MPN: 0353630460</t>
   </si>
   <si>
-    <t>Yes (encoder connectors)</t>
-  </si>
-  <si>
     <t>4.7k</t>
   </si>
   <si>
@@ -289,9 +268,6 @@
     <t>J3</t>
   </si>
   <si>
-    <t>Needs replacement</t>
-  </si>
-  <si>
     <t>68k</t>
   </si>
   <si>
@@ -313,9 +289,6 @@
     <t>DD:J1</t>
   </si>
   <si>
-    <t>Yes (Dribbler motor connector)</t>
-  </si>
-  <si>
     <t>94HCB16T</t>
   </si>
   <si>
@@ -343,12 +316,6 @@
     <t>APA102C 5050 RGB LED</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Direct substitute: BL-HBGR32L-3-TRB-8</t>
-  </si>
-  <si>
     <t>ASV-18.432MHZ-EJ-T</t>
   </si>
   <si>
@@ -379,9 +346,6 @@
     <t>J6</t>
   </si>
   <si>
-    <t>Replace with XT-60 Connector</t>
-  </si>
-  <si>
     <t>DRV8303DCA</t>
   </si>
   <si>
@@ -391,9 +355,6 @@
     <t>DD:U1, M1:U1, M2:U1, M3:U1, M4:U1</t>
   </si>
   <si>
-    <t>No, replace</t>
-  </si>
-  <si>
     <t>ECA-1HHG221</t>
   </si>
   <si>
@@ -427,9 +388,6 @@
     <t>J1, J2, J4</t>
   </si>
   <si>
-    <t>Replace</t>
-  </si>
-  <si>
     <t>IMUIMU-KIT</t>
   </si>
   <si>
@@ -442,9 +400,6 @@
     <t>IMU breakout board</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>IRFH7545</t>
   </si>
   <si>
@@ -548,85 +503,13 @@
   </si>
   <si>
     <t>Spartan-3E 144pin</t>
-  </si>
-  <si>
-    <t>Replacement: XT60PW-M</t>
-  </si>
-  <si>
-    <t>Replacement: DRV8301DCAR (extremely similar, slight changes)</t>
-  </si>
-  <si>
-    <t>Replacement: SFW8R-2STAE1LF</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/amphenol-cs-fci/SFW8S-2STAE1LF/4271116</t>
-  </si>
-  <si>
-    <t>Replacement: SFW8S-2STAE1LF</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/littelfuse-inc/0805L200SLTHYR/3661958?s=N4IgTCBcDaIAwA44FYAyY5wMqoCoAkBNAJRAF0BfIA</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/keystone-electronics/3557-2/2137305</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/grayhill-inc/34EWMSP12M6RT/2679145?s=N4IgTCBcDaIMwBYCiB1AsgZQAoEYxoDYAlAFRAF0BfIA</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/molex/0353630460/736076?s=N4IgTCBcDaIAwGYCsCBsC4BZVxAXQF8g</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/molex/0353630860/755312?s=N4IgTCBcDaIOoFkCMAOAnAZgOwFoByAIiALoC%2BQA</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/american-bright-optoelectronics-corporation/BL-HBGR32L-3-TRB-8/9817409?s=N4IgTCBcDaIEIBkC0AJOBxASgZjM7SAKpnEgBwgC6AvkA</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/en/details/xt60pw-m/dc-power-connectors/amass/</t>
-  </si>
-  <si>
-    <t>Link To Part (Or Replacement)</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/DRV8301DCAR?qs=SMj%252Bbyv09TwYHebRFanjcw%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/SFW8R-2STAE1LF/609-SFW8R-2STAE1LFCT-ND/12760962?curr=usd&amp;utm_campaign=buynow&amp;utm_medium=aggregator&amp;utm_source=octopart</t>
-  </si>
-  <si>
-    <t>Check shop for spares</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/MPM3620GQV-P/1589-1252-1-ND/5298339?curr=usd&amp;utm_campaign=buynow&amp;utm_medium=aggregator&amp;utm_source=octopart</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Infineon-Technologies/IRFH7545TRPBF?qs=NBFAU1oqP4Xy0KalJOxHdQ%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.arrow.com/en/products/mcp1824t-1202eot/microchip-technology?region=nac&amp;utm_campaign=octopart_2022&amp;utm_content=inv_listing&amp;utm_currency=USD&amp;utm_keyword=MCP1824T-1202E%2FOT&amp;utm_medium=aggregator&amp;utm_source=octopart</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/MCP1824T-2502E-OT/MCP1824T-2502E-OTCT-ND/1817326?curr=usd&amp;utm_campaign=buynow&amp;utm_medium=aggregator&amp;utm_source=octopart</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/ASV-1.8432MHZ-EJ-T/535-9315-1-ND/675736?curr=usd&amp;utm_campaign=buynow&amp;utm_medium=aggregator&amp;utm_source=octopart</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/BSS806NH6327XTSA1/BSS806NH6327XTSA1CT-ND/3196655?curr=usd&amp;utm_campaign=buynow&amp;utm_medium=aggregator&amp;utm_source=octopart</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/ECA-1HHG221/245171</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -761,14 +644,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1067,7 +942,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1110,13 +985,11 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1150,7 +1023,6 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1175,18 +1047,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I55" totalsRowShown="0">
-  <autoFilter ref="A1:I55"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="Qty"/>
-    <tableColumn id="2" name="Value"/>
-    <tableColumn id="3" name="Device"/>
-    <tableColumn id="4" name="Package"/>
-    <tableColumn id="5" name="Parts"/>
-    <tableColumn id="6" name="Description"/>
-    <tableColumn id="7" name="Availability"/>
-    <tableColumn id="8" name="Replacement/Action"/>
-    <tableColumn id="9" name="Link To Part (Or Replacement)"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:F55" totalsRowShown="0">
+  <autoFilter ref="A1:F55" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Qty"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Device"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Package"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parts"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1488,11 +1357,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1501,12 +1370,9 @@
     <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.140625" customWidth="1"/>
     <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="130" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1525,17 +1391,8 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4</v>
       </c>
@@ -1543,519 +1400,393 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" t="s">
-        <v>196</v>
-      </c>
-      <c r="I6" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
         <v>9</v>
       </c>
-      <c r="E8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
         <v>9</v>
       </c>
-      <c r="E11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" t="s">
         <v>9</v>
       </c>
-      <c r="E12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>39</v>
       </c>
-      <c r="F13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="F14" t="s">
         <v>40</v>
       </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" t="s">
-        <v>44</v>
-      </c>
-      <c r="H14" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
       <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
         <v>45</v>
       </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F16" t="s">
         <v>46</v>
       </c>
-      <c r="F15" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" t="s">
-        <v>51</v>
-      </c>
-      <c r="H16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
         <v>53</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
         <v>54</v>
       </c>
-      <c r="D17" t="s">
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
         <v>55</v>
       </c>
-      <c r="E17" t="s">
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
         <v>56</v>
       </c>
-      <c r="F17" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
         <v>57</v>
       </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="C21" t="s">
         <v>58</v>
       </c>
-      <c r="F18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" t="s">
         <v>59</v>
       </c>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21" t="s">
-        <v>65</v>
-      </c>
-      <c r="G21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" t="s">
-        <v>196</v>
-      </c>
-      <c r="I21" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2063,25 +1794,19 @@
         <v>330</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" t="s">
         <v>9</v>
       </c>
-      <c r="E22" t="s">
-        <v>66</v>
-      </c>
-      <c r="F22" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>9</v>
       </c>
@@ -2089,819 +1814,612 @@
         <v>330</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D23" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F23" t="s">
-        <v>70</v>
-      </c>
-      <c r="G23" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D24" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E24" t="s">
-        <v>72</v>
-      </c>
-      <c r="G24" t="s">
-        <v>12</v>
-      </c>
-      <c r="H24" t="s">
-        <v>196</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E25" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F25" t="s">
-        <v>76</v>
-      </c>
-      <c r="G25" t="s">
-        <v>77</v>
-      </c>
-      <c r="H25" t="s">
-        <v>196</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
       <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
         <v>78</v>
       </c>
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="F29" t="s">
         <v>9</v>
       </c>
-      <c r="E26" t="s">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
         <v>79</v>
       </c>
-      <c r="F26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26" t="s">
-        <v>12</v>
-      </c>
-      <c r="H26" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="C30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" t="s">
         <v>80</v>
       </c>
-      <c r="C27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" t="s">
         <v>9</v>
       </c>
-      <c r="E27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>82</v>
-      </c>
-      <c r="C28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" t="s">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" t="s">
         <v>9</v>
       </c>
-      <c r="E28" t="s">
-        <v>83</v>
-      </c>
-      <c r="F28" t="s">
-        <v>11</v>
-      </c>
-      <c r="G28" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" t="s">
-        <v>85</v>
-      </c>
-      <c r="F29" t="s">
-        <v>11</v>
-      </c>
-      <c r="G29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
         <v>86</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C33" t="s">
         <v>86</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D33" t="s">
         <v>87</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E33" t="s">
         <v>88</v>
       </c>
-      <c r="G30" t="s">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
         <v>89</v>
       </c>
-      <c r="H30" t="s">
-        <v>180</v>
-      </c>
-      <c r="I30" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="C34" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" t="s">
         <v>90</v>
       </c>
-      <c r="C31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="E34" t="s">
         <v>91</v>
       </c>
-      <c r="F31" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="F34" t="s">
         <v>92</v>
       </c>
-      <c r="C32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" t="s">
-        <v>93</v>
-      </c>
-      <c r="F32" t="s">
-        <v>11</v>
-      </c>
-      <c r="G32" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>1</v>
-      </c>
-      <c r="B33" t="s">
-        <v>94</v>
-      </c>
-      <c r="C33" t="s">
-        <v>94</v>
-      </c>
-      <c r="D33" t="s">
-        <v>95</v>
-      </c>
-      <c r="E33" t="s">
-        <v>96</v>
-      </c>
-      <c r="G33" t="s">
-        <v>97</v>
-      </c>
-      <c r="H33" t="s">
-        <v>196</v>
-      </c>
-      <c r="I33" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>1</v>
-      </c>
-      <c r="B34" t="s">
-        <v>98</v>
-      </c>
-      <c r="C34" t="s">
-        <v>98</v>
-      </c>
-      <c r="D34" t="s">
-        <v>99</v>
-      </c>
-      <c r="E34" t="s">
-        <v>100</v>
-      </c>
-      <c r="F34" t="s">
-        <v>101</v>
-      </c>
-      <c r="G34" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C35" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D35" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E35" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F35" t="s">
-        <v>106</v>
-      </c>
-      <c r="G35" t="s">
-        <v>107</v>
-      </c>
-      <c r="H35" t="s">
-        <v>108</v>
-      </c>
-      <c r="I35" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C36" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="D36" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="E36" t="s">
-        <v>111</v>
-      </c>
-      <c r="G36" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" t="s">
-        <v>196</v>
-      </c>
-      <c r="I36" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C37" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D37" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="E37" t="s">
-        <v>115</v>
-      </c>
-      <c r="G37" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" t="s">
-        <v>196</v>
-      </c>
-      <c r="I37" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C38" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="D38" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="E38" t="s">
-        <v>118</v>
-      </c>
-      <c r="G38" t="s">
-        <v>119</v>
-      </c>
-      <c r="H38" t="s">
-        <v>176</v>
-      </c>
-      <c r="I38" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C39" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="D39" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="E39" t="s">
-        <v>122</v>
-      </c>
-      <c r="G39" t="s">
-        <v>123</v>
-      </c>
-      <c r="H39" t="s">
-        <v>177</v>
-      </c>
-      <c r="I39" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="C40" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="D40" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="E40" t="s">
-        <v>126</v>
-      </c>
-      <c r="G40" t="s">
-        <v>12</v>
-      </c>
-      <c r="H40" t="s">
-        <v>196</v>
-      </c>
-      <c r="I40" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C41" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="D41" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="E41" t="s">
-        <v>130</v>
-      </c>
-      <c r="G41" t="s">
-        <v>12</v>
-      </c>
-      <c r="H41" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" t="s">
+        <v>119</v>
+      </c>
+      <c r="F42" t="s">
         <v>14</v>
       </c>
-      <c r="D42" t="s">
-        <v>15</v>
-      </c>
-      <c r="E42" t="s">
-        <v>132</v>
-      </c>
-      <c r="F42" t="s">
-        <v>17</v>
-      </c>
-      <c r="G42" t="s">
-        <v>12</v>
-      </c>
-      <c r="H42" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="C43" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="D43" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="E43" t="s">
-        <v>134</v>
-      </c>
-      <c r="G43" t="s">
-        <v>135</v>
-      </c>
-      <c r="H43" t="s">
-        <v>178</v>
-      </c>
-      <c r="I43" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="C44" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="D44" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="E44" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="F44" t="s">
-        <v>139</v>
-      </c>
-      <c r="G44" t="s">
-        <v>140</v>
-      </c>
-      <c r="H44" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>30</v>
       </c>
       <c r="B45" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="C45" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="D45" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E45" t="s">
-        <v>143</v>
-      </c>
-      <c r="G45" t="s">
-        <v>12</v>
-      </c>
-      <c r="H45" t="s">
-        <v>196</v>
-      </c>
-      <c r="I45" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="C46" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="D46" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="E46" t="s">
-        <v>146</v>
-      </c>
-      <c r="G46" t="s">
-        <v>12</v>
-      </c>
-      <c r="H46" t="s">
-        <v>196</v>
-      </c>
-      <c r="I46" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="C47" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="D47" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="E47" t="s">
-        <v>148</v>
-      </c>
-      <c r="G47" t="s">
-        <v>12</v>
-      </c>
-      <c r="H47" t="s">
-        <v>196</v>
-      </c>
-      <c r="I47" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="C48" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="D48" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="E48" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="F48" t="s">
-        <v>152</v>
-      </c>
-      <c r="G48" t="s">
-        <v>107</v>
-      </c>
-      <c r="H48" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="C49" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="D49" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="E49" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="C50" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="D50" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="E50" t="s">
-        <v>156</v>
-      </c>
-      <c r="G50" t="s">
-        <v>12</v>
-      </c>
-      <c r="I50" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="C51" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="D51" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="E51" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="F51" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C52" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="D52" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="E52" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="C53" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="D53" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="E53" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="F53" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="C54" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="D54" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="E54" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="C55" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="D55" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="E55" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="F55" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I25" r:id="rId1"/>
-    <hyperlink ref="I24" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>